<commit_message>
UC Time Estimation first draft updated
</commit_message>
<xml_diff>
--- a/documentation/RiskManagement.xlsx
+++ b/documentation/RiskManagement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Service\Desktop\PerfectTimeWorkspace\PerfectTime\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4287222-EAD4-43F0-8018-5DF4D5FFABA1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCBF95F9-114C-47E8-9CD3-5B57127EA055}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C04EA984-3C12-41AE-8DB7-D5A135D3159D}"/>
   </bookViews>
@@ -393,6 +393,162 @@
   </cellStyles>
   <dxfs count="11">
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -421,162 +577,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -591,18 +591,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F0BEEBFE-7FD8-40F5-8BAB-6889FDCBB521}" name="Tabelle1" displayName="Tabelle1" ref="A6:G12" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="9" tableBorderDxfId="10" totalsRowBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F0BEEBFE-7FD8-40F5-8BAB-6889FDCBB521}" name="Tabelle1" displayName="Tabelle1" ref="A6:G12" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8" totalsRowBorderDxfId="7">
   <autoFilter ref="A6:G12" xr:uid="{580D1EA3-22A1-4444-A7A5-65912A5AAA0B}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{889317FF-A62A-4870-B8D1-DC8A146631A1}" name="Risk Name" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{9BCEA6D7-C24A-49C4-B496-15BD6931516D}" name="Risk Description" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{6EC3FA39-BE0F-478E-A04D-A423C5626B30}" name="Risk Probability _x000a_of Occurrence (in %)" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{2D1C35A6-A540-4854-95D9-848DCBF0BFA7}" name="Risk Impact _x000a_(1 low - 10 extreme)" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{1E44A2D3-DBAC-4E4D-A9EC-7181A63C6B2B}" name="Risk Factor" dataDxfId="3">
+    <tableColumn id="1" xr3:uid="{889317FF-A62A-4870-B8D1-DC8A146631A1}" name="Risk Name" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{9BCEA6D7-C24A-49C4-B496-15BD6931516D}" name="Risk Description" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{6EC3FA39-BE0F-478E-A04D-A423C5626B30}" name="Risk Probability _x000a_of Occurrence (in %)" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{2D1C35A6-A540-4854-95D9-848DCBF0BFA7}" name="Risk Impact _x000a_(1 low - 10 extreme)" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{1E44A2D3-DBAC-4E4D-A9EC-7181A63C6B2B}" name="Risk Factor" dataDxfId="2">
       <calculatedColumnFormula>C7*D7</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{1B57ADC3-CE5E-4AE0-BC87-7D435D391C3B}" name="Risk Mitigation _x000a_(Measures)" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{0D4E0051-AE46-44F5-B3F5-C584BF5FB65D}" name="Person in Charge of Tracking _x000a_(not person who brought it up!!) " dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{1B57ADC3-CE5E-4AE0-BC87-7D435D391C3B}" name="Risk Mitigation _x000a_(Measures)" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{0D4E0051-AE46-44F5-B3F5-C584BF5FB65D}" name="Person in Charge of Tracking _x000a_(not person who brought it up!!) " dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -907,8 +907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{930ADE0A-524A-4165-A099-062AA5CBAC8D}">
   <dimension ref="A2:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -918,7 +918,7 @@
     <col min="3" max="4" width="22.85546875" customWidth="1"/>
     <col min="5" max="5" width="22.7109375" customWidth="1"/>
     <col min="6" max="6" width="33.140625" customWidth="1"/>
-    <col min="7" max="7" width="23" customWidth="1"/>
+    <col min="7" max="7" width="25.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
@@ -973,7 +973,7 @@
         <v>10</v>
       </c>
       <c r="E7" s="3">
-        <f>C7*D7</f>
+        <f t="shared" ref="E7:E12" si="0">C7*D7</f>
         <v>1.5</v>
       </c>
       <c r="F7" s="4" t="s">
@@ -997,7 +997,7 @@
         <v>3</v>
       </c>
       <c r="E8" s="3">
-        <f>C8*D8</f>
+        <f t="shared" si="0"/>
         <v>1.2000000000000002</v>
       </c>
       <c r="F8" s="4" t="s">
@@ -1021,7 +1021,7 @@
         <v>5</v>
       </c>
       <c r="E9" s="3">
-        <f>C9*D9</f>
+        <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
       <c r="F9" s="4" t="s">
@@ -1045,7 +1045,7 @@
         <v>3</v>
       </c>
       <c r="E10" s="3">
-        <f>C10*D10</f>
+        <f t="shared" si="0"/>
         <v>0.60000000000000009</v>
       </c>
       <c r="F10" s="4" t="s">
@@ -1069,7 +1069,7 @@
         <v>9</v>
       </c>
       <c r="E11" s="3">
-        <f>C11*D11</f>
+        <f t="shared" si="0"/>
         <v>0.18</v>
       </c>
       <c r="F11" s="4" t="s">
@@ -1093,7 +1093,7 @@
         <v>3</v>
       </c>
       <c r="E12" s="14">
-        <f>C12*D12</f>
+        <f t="shared" si="0"/>
         <v>0.03</v>
       </c>
       <c r="F12" s="15" t="s">

</xml_diff>

<commit_message>
Updated SAD with container pattern and Risks
</commit_message>
<xml_diff>
--- a/documentation/RiskManagement.xlsx
+++ b/documentation/RiskManagement.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Service\Desktop\PerfectTimeWorkspace\PerfectTime\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9210BD54-8E14-42E3-84E7-942B3BFC8A67}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C9E51BE-F5C7-4C1A-988F-1DC43477D05A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C04EA984-3C12-41AE-8DB7-D5A135D3159D}"/>
   </bookViews>
@@ -907,8 +907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{930ADE0A-524A-4165-A099-062AA5CBAC8D}">
   <dimension ref="A2:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -967,14 +967,14 @@
         <v>15</v>
       </c>
       <c r="C7" s="2">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
       <c r="D7" s="3">
         <v>10</v>
       </c>
       <c r="E7" s="3">
         <f t="shared" ref="E7:E12" si="0">C7*D7</f>
-        <v>1.5</v>
+        <v>1.6</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>27</v>
@@ -991,14 +991,14 @@
         <v>16</v>
       </c>
       <c r="C8" s="2">
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
       <c r="D8" s="3">
         <v>3</v>
       </c>
       <c r="E8" s="3">
         <f t="shared" si="0"/>
-        <v>1.0499999999999998</v>
+        <v>0.89999999999999991</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>28</v>
@@ -1015,14 +1015,14 @@
         <v>18</v>
       </c>
       <c r="C9" s="2">
-        <v>0.15</v>
+        <v>0.12</v>
       </c>
       <c r="D9" s="3">
         <v>6</v>
       </c>
       <c r="E9" s="3">
         <f t="shared" si="0"/>
-        <v>0.89999999999999991</v>
+        <v>0.72</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>30</v>
@@ -1039,14 +1039,14 @@
         <v>19</v>
       </c>
       <c r="C10" s="2">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
       <c r="D10" s="3">
         <v>3</v>
       </c>
       <c r="E10" s="3">
         <f t="shared" si="0"/>
-        <v>0.75</v>
+        <v>0.60000000000000009</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>31</v>
@@ -1063,14 +1063,14 @@
         <v>17</v>
       </c>
       <c r="C11" s="2">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="D11" s="3">
         <v>9</v>
       </c>
       <c r="E11" s="3">
         <f t="shared" si="0"/>
-        <v>0.18</v>
+        <v>0.09</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
Preparations for hand in
</commit_message>
<xml_diff>
--- a/documentation/RiskManagement.xlsx
+++ b/documentation/RiskManagement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Service\Desktop\PerfectTimeWorkspace\PerfectTime\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C9E51BE-F5C7-4C1A-988F-1DC43477D05A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41353A3C-7ECF-4870-905C-FA9A537157C4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C04EA984-3C12-41AE-8DB7-D5A135D3159D}"/>
   </bookViews>
@@ -907,8 +907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{930ADE0A-524A-4165-A099-062AA5CBAC8D}">
   <dimension ref="A2:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -967,14 +967,14 @@
         <v>15</v>
       </c>
       <c r="C7" s="2">
-        <v>0.16</v>
+        <v>0.18</v>
       </c>
       <c r="D7" s="3">
         <v>10</v>
       </c>
       <c r="E7" s="3">
         <f t="shared" ref="E7:E12" si="0">C7*D7</f>
-        <v>1.6</v>
+        <v>1.7999999999999998</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>27</v>
@@ -991,14 +991,14 @@
         <v>16</v>
       </c>
       <c r="C8" s="2">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="D8" s="3">
         <v>3</v>
       </c>
       <c r="E8" s="3">
         <f t="shared" si="0"/>
-        <v>0.89999999999999991</v>
+        <v>0.60000000000000009</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>28</v>
@@ -1015,14 +1015,14 @@
         <v>18</v>
       </c>
       <c r="C9" s="2">
-        <v>0.12</v>
+        <v>0.1</v>
       </c>
       <c r="D9" s="3">
         <v>6</v>
       </c>
       <c r="E9" s="3">
         <f t="shared" si="0"/>
-        <v>0.72</v>
+        <v>0.60000000000000009</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>30</v>
@@ -1039,14 +1039,14 @@
         <v>19</v>
       </c>
       <c r="C10" s="2">
-        <v>0.2</v>
+        <v>0.18</v>
       </c>
       <c r="D10" s="3">
         <v>3</v>
       </c>
       <c r="E10" s="3">
         <f t="shared" si="0"/>
-        <v>0.60000000000000009</v>
+        <v>0.54</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>31</v>
@@ -1087,14 +1087,14 @@
         <v>20</v>
       </c>
       <c r="C12" s="13">
-        <v>0.01</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="D12" s="14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E12" s="14">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>0.01</v>
       </c>
       <c r="F12" s="15" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
Updated documents with time spent for final hand in
Presentation, Report, Risk and Time calc
</commit_message>
<xml_diff>
--- a/documentation/RiskManagement.xlsx
+++ b/documentation/RiskManagement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Service\Desktop\PerfectTimeWorkspace\PerfectTime\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41353A3C-7ECF-4870-905C-FA9A537157C4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E2E8697-1B73-4A91-AB58-E341FC13210C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C04EA984-3C12-41AE-8DB7-D5A135D3159D}"/>
   </bookViews>
@@ -907,7 +907,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{930ADE0A-524A-4165-A099-062AA5CBAC8D}">
   <dimension ref="A2:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -983,76 +983,76 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C8" s="2">
-        <v>0.2</v>
+        <v>0.09</v>
       </c>
       <c r="D8" s="3">
+        <v>6</v>
+      </c>
+      <c r="E8" s="3">
+        <f>C8*D8</f>
+        <v>0.54</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="D9" s="3">
         <v>3</v>
-      </c>
-      <c r="E8" s="3">
-        <f t="shared" si="0"/>
-        <v>0.60000000000000009</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="D9" s="3">
-        <v>6</v>
       </c>
       <c r="E9" s="3">
         <f t="shared" si="0"/>
-        <v>0.60000000000000009</v>
+        <v>0.44999999999999996</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C10" s="2">
-        <v>0.18</v>
+        <v>0.03</v>
       </c>
       <c r="D10" s="3">
         <v>3</v>
       </c>
       <c r="E10" s="3">
-        <f t="shared" si="0"/>
-        <v>0.54</v>
+        <f>C10*D10</f>
+        <v>0.09</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="75" x14ac:dyDescent="0.25">

</xml_diff>